<commit_message>
Ajout de Gerber Files
</commit_message>
<xml_diff>
--- a/Matériel/plan de test PCB mallette.xlsx
+++ b/Matériel/plan de test PCB mallette.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\OneDrive\Documents\GitHub\Projet Final TSO\Projet_Final_TSO\Matériel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B510EC9-C934-4B8B-BCCD-40763AFD131C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CE9D3D-A7CF-4319-8EAE-17F236C5CD37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{CF7E7B00-0B90-4AA1-96DC-F02D56B415EB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CF7E7B00-0B90-4AA1-96DC-F02D56B415EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>Fonction</t>
   </si>
@@ -104,12 +104,6 @@
     <t>Tester pour les court-circuits avec un multimètre en mode résistance sur les pattes 5v et mise à terre</t>
   </si>
   <si>
-    <t>Tester la résistance entre les pattes des composants énergivores avec un multimètre en mode résistance sur les pattes 5v et la patte des pattes des Vin des composantes.</t>
-  </si>
-  <si>
-    <t>Tester l'ergonomique de la poignée. Verifier s'il y a des angles coupants</t>
-  </si>
-  <si>
     <t>Mécanique</t>
   </si>
   <si>
@@ -119,9 +113,6 @@
     <t>Connecteur USB-C</t>
   </si>
   <si>
-    <t>Le PCB est fonctionnel du bon coté selon l'indication sur le silkcreen</t>
-  </si>
-  <si>
     <t>Dimension de la mallette et du PCB</t>
   </si>
   <si>
@@ -171,6 +162,18 @@
   </si>
   <si>
     <t>Avec le programme python "integrationTotal" vérifier que tout les esp32 et leurs objets interactifs transmettent leurs donnèes et les affichent sur le mini écran.</t>
+  </si>
+  <si>
+    <t>Tester la résistance entre les pattes des composants énergivores avec un multimètre en mode résistance sur les pattes 5v et les pattes des Vin des composantes.</t>
+  </si>
+  <si>
+    <t>Tester l'ergonomie de la poignée. Verifier s'il y a des angles coupants</t>
+  </si>
+  <si>
+    <t>Problème de fabrication, il n'y pas de poigné</t>
+  </si>
+  <si>
+    <t>Le USB-C est fonctionnel du bon coté selon l'indication sur le silkcreen</t>
   </si>
 </sst>
 </file>
@@ -498,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -599,7 +602,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1148,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A179C3DD-CE59-450A-90EC-B70C1216426A}">
   <dimension ref="B1:G42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1203,7 +1205,7 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1270,40 +1272,46 @@
         <v>20</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="22"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="15"/>
+        <v>43</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>44</v>
+      </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="2:7" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="28" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="19"/>
+        <v>23</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="E13" s="22"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="15"/>
@@ -1311,32 +1319,36 @@
     </row>
     <row r="15" spans="2:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="19"/>
+        <v>26</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="E15" s="22"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="2:7" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="36" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="19"/>
+        <v>29</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="E16" s="15"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="2:6" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="28" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="22"/>
@@ -1344,10 +1356,10 @@
     </row>
     <row r="18" spans="2:6" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="36" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="22"/>
@@ -1355,10 +1367,10 @@
     </row>
     <row r="19" spans="2:6" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="28" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="15"/>
@@ -1366,10 +1378,10 @@
     </row>
     <row r="20" spans="2:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D20" s="19"/>
       <c r="E20" s="15"/>
@@ -1377,10 +1389,10 @@
     </row>
     <row r="21" spans="2:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="28" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="22"/>
@@ -1388,10 +1400,10 @@
     </row>
     <row r="22" spans="2:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="15"/>

</xml_diff>